<commit_message>
Improve Exception Handling Fix a couple of bugs
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="465" windowWidth="26220" windowHeight="10815" tabRatio="714" activeTab="10"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="26220" windowHeight="10815" tabRatio="714" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -791,33 +791,6 @@
     <t>Description=Dummy Tests With Errors;EmailBody=This test should FAIL big time</t>
   </si>
   <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:Calculate</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:ChainingFinders</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:CssFinders</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:FrameSwitching</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:Dummy Tests</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:Dummy Tests Errors</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:DoCalculate</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:DoChain</t>
-  </si>
-  <si>
-    <t>InputSpecs=File:DDTRoot.xlsx:DoCssFinder</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">This spreadsheet leverages </t>
     </r>
@@ -842,6 +815,33 @@
       </rPr>
       <t xml:space="preserve"> test website - a web site that is the 'test lab' of his (EXCELLENT) course on Web Testing.</t>
     </r>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!Calculate</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!ChainingFinders</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!CssFinders</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!FrameSwitching</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!Dummy Tests</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!Dummy Tests Errors</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!DoCalculate</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!DoChain</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!DoCssFinder</t>
   </si>
 </sst>
 </file>
@@ -2703,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2719,10 +2719,11 @@
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
     <col min="7" max="7" width="62" style="1" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="51.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2756,13 +2757,17 @@
         <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTDemo01",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!Calculate",  "Run the Calculator tests"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2770,13 +2775,17 @@
         <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I8" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTDemo02",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!ChainingFinders",  "Run the ChainFinders tests"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2784,13 +2793,17 @@
         <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"DDTDemo03",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!CssFinders",  "Run the CssFinders tests"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
@@ -2798,13 +2811,17 @@
         <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"DDTDemo04",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!FrameSwitching",  "Run the Frame Switching tests"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>139</v>
       </c>
@@ -2812,13 +2829,17 @@
         <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"DummyTestPass01",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!Dummy Tests",  "Run Dummy Tests - No Web Driver involved"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>140</v>
       </c>
@@ -2826,13 +2847,17 @@
         <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"DummyTestFail01",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!Dummy Tests Errors",  "Run Dummy Tests - No Web Driver involved"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>200</v>
       </c>
@@ -2844,6 +2869,10 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>187</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"DDTDemo05",  "generateReport",  "",  "",  "",  "",  "Description=Summary Report",  "DDT Tests"});</v>
       </c>
     </row>
   </sheetData>
@@ -2870,10 +2899,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2884,9 +2913,10 @@
     <col min="4" max="5" width="10" customWidth="1"/>
     <col min="7" max="7" width="86.42578125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>173</v>
       </c>
@@ -2929,8 +2959,12 @@
       <c r="H2" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr01",  "verify",  "",  "",  "",  "",  "Value=12345;ActualValue=23456;Class=Int;CompareMode=&lt;",  "Dummy Integer test"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>174</v>
       </c>
@@ -2947,8 +2981,12 @@
       <c r="H3" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr02",  "verify",  "",  "",  "",  "",  "Value=-12,345;ActualValue=23,456,456,789;Class=Long;CompareMode=Equals",  "Dummy Long test"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>175</v>
       </c>
@@ -2965,8 +3003,12 @@
       <c r="H4" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr03",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001;ActualValue=23,456,456,789.00007;Class=Decimal;CompareMode=GT",  "Dummy Decimal test"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>176</v>
       </c>
@@ -2983,8 +3025,12 @@
       <c r="H5" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr04",  "verify",  "",  "",  "",  "",  "Value=$12,345;ActualValue=$23,456;Class=Amount;CompareMode=LessThan",  "Dummy Currency test"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>177</v>
       </c>
@@ -3001,8 +3047,12 @@
       <c r="H6" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr05",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001;ActualValue=;Class=Decimal;CompareMode=empty",  "Dummy Decimal test"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>178</v>
       </c>
@@ -3019,8 +3069,12 @@
       <c r="H7" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr06",  "verify",  "",  "",  "",  "",  "Value=02/03/2000;ActualValue=03/02/2010;Class=Date;CompareMode=before;Option=MM/dd/yyyy",  "Dummy Date test"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>179</v>
       </c>
@@ -3037,8 +3091,12 @@
       <c r="H8" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr07",  "verify",  "",  "",  "",  "",  "Value=02/03/2000.and.05/05/2009;ActualValue=03/02/2010;Class=Date;CompareMode=between;Option=MM/dd/yyyy",  "Test date between early and late date"});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>190</v>
       </c>
@@ -3055,8 +3113,12 @@
       <c r="H9" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr08",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001.and.23,456;ActualValue=100,000.05;Class=Decimal;CompareMode=Between",  "Dummy Decimal Between test"});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>191</v>
       </c>
@@ -3073,8 +3135,12 @@
       <c r="H10" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A10 &amp; """" &amp; ",  " &amp; """" &amp; B10 &amp; """" &amp; ",  " &amp; """" &amp; C10 &amp; """" &amp; ",  " &amp; """" &amp; D10 &amp;  """" &amp;  ",  " &amp; """" &amp; E10 &amp; """" &amp; ",  " &amp; """" &amp; F10 &amp; """" &amp; ",  " &amp; """" &amp; G10 &amp; """" &amp; ",  " &amp; """" &amp; H10 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr09",  "verify",  "",  "",  "",  "",  "Value=-12,345.and.23,456;ActualValue=100,000;Class=Long;CompareMode=Between",  "Dummy Long (between) test"});</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>194</v>
       </c>
@@ -3091,8 +3157,12 @@
       <c r="H11" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A11 &amp; """" &amp; ",  " &amp; """" &amp; B11 &amp; """" &amp; ",  " &amp; """" &amp; C11 &amp; """" &amp; ",  " &amp; """" &amp; D11 &amp;  """" &amp;  ",  " &amp; """" &amp; E11 &amp; """" &amp; ",  " &amp; """" &amp; F11 &amp; """" &amp; ",  " &amp; """" &amp; G11 &amp; """" &amp; ",  " &amp; """" &amp; H11 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr10",  "verify",  "",  "",  "",  "",  "Value=-12,345.and.23,456;ActualValue=32767;Class=Integer;CompareMode=Between",  "Dummy Integer (between) test"});</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>195</v>
       </c>
@@ -3109,8 +3179,12 @@
       <c r="H12" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A12 &amp; """" &amp; ",  " &amp; """" &amp; B12 &amp; """" &amp; ",  " &amp; """" &amp; C12 &amp; """" &amp; ",  " &amp; """" &amp; D12 &amp;  """" &amp;  ",  " &amp; """" &amp; E12 &amp; """" &amp; ",  " &amp; """" &amp; F12 &amp; """" &amp; ",  " &amp; """" &amp; G12 &amp; """" &amp; ",  " &amp; """" &amp; H12 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr11",  "verify",  "",  "",  "",  "",  "Value=abc.and.def;ActualValue=bcd;CompareMode=Between",  "Dummy Strings (between) test"});</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>199</v>
       </c>
@@ -3126,6 +3200,10 @@
       </c>
       <c r="H13" s="1" t="s">
         <v>137</v>
+      </c>
+      <c r="I13" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A13 &amp; """" &amp; ",  " &amp; """" &amp; B13 &amp; """" &amp; ",  " &amp; """" &amp; C13 &amp; """" &amp; ",  " &amp; """" &amp; D13 &amp;  """" &amp;  ",  " &amp; """" &amp; E13 &amp; """" &amp; ",  " &amp; """" &amp; F13 &amp; """" &amp; ",  " &amp; """" &amp; G13 &amp; """" &amp; ",  " &amp; """" &amp; H13 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"VerifyErr12",  "generateReport",  "",  "",  "",  "",  "Description=Dummy Tests With Errors;EmailBody=This test should FAIL big time",  "Generate Dummy Tests Report (Errors)"});</v>
       </c>
     </row>
   </sheetData>
@@ -3169,7 +3247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3198,7 +3276,7 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3229,10 +3307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I2" sqref="I2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3244,10 +3322,11 @@
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
     <col min="7" max="7" width="47.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="54.85546875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3273,7 +3352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -3286,8 +3365,12 @@
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+      <c r="I2" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate01",  "setVars",  "",  "",  "",  "",  "URL=http://compendiumdev.co.uk/selenium/calculate.php;BaseTitle=The "Selenium Simplified" Calculator",  "Set the Browser and Base URL - TODO: Resolve issue with Browser Type"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -3300,8 +3383,12 @@
       <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
+      <c r="I3" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate02",  "createWebDriver",  "",  "",  "",  "",  "URL={url}",  "Launch the Browser with base URL"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -3314,8 +3401,12 @@
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+      <c r="I4" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate03",  "setVars",  "",  "",  "",  "",  "Number1=1;Number2=2;Action=plus;Answer=33;Function=GetText;CompareMode=NotBlank",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -3323,13 +3414,17 @@
         <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15">
+      <c r="I5" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate04",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -3342,8 +3437,12 @@
       <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
+      <c r="I6" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate05",  "setVars",  "",  "",  "",  "",  "Number1=2;Number2=1;Action=minus;Answer=1;Function=GetText;CompareMode=Is",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -3351,13 +3450,17 @@
         <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+      <c r="I7" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate06",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3370,8 +3473,12 @@
       <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15">
+      <c r="I8" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate07",  "setVars",  "",  "",  "",  "",  "Number1=1234;Number2=11;Action=times;Answer=574;Function=GetText;CompareMode=EndsWith",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -3379,13 +3486,17 @@
         <v>102</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15">
+      <c r="I9" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate08",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -3398,8 +3509,12 @@
       <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15">
+      <c r="I10" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A10 &amp; """" &amp; ",  " &amp; """" &amp; B10 &amp; """" &amp; ",  " &amp; """" &amp; C10 &amp; """" &amp; ",  " &amp; """" &amp; D10 &amp;  """" &amp;  ",  " &amp; """" &amp; E10 &amp; """" &amp; ",  " &amp; """" &amp; F10 &amp; """" &amp; ",  " &amp; """" &amp; G10 &amp; """" &amp; ",  " &amp; """" &amp; H10 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate09",  "setVars",  "",  "",  "",  "",  "Number1=1234;Number2=11;Action=times;Answer=1.*4;Function=GetText;CompareMode=Matches",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -3407,13 +3522,17 @@
         <v>102</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15">
+      <c r="I11" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A11 &amp; """" &amp; ",  " &amp; """" &amp; B11 &amp; """" &amp; ",  " &amp; """" &amp; C11 &amp; """" &amp; ",  " &amp; """" &amp; D11 &amp;  """" &amp;  ",  " &amp; """" &amp; E11 &amp; """" &amp; ",  " &amp; """" &amp; F11 &amp; """" &amp; ",  " &amp; """" &amp; G11 &amp; """" &amp; ",  " &amp; """" &amp; H11 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate10",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -3426,8 +3545,12 @@
       <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15">
+      <c r="I12" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A12 &amp; """" &amp; ",  " &amp; """" &amp; B12 &amp; """" &amp; ",  " &amp; """" &amp; C12 &amp; """" &amp; ",  " &amp; """" &amp; D12 &amp;  """" &amp;  ",  " &amp; """" &amp; E12 &amp; """" &amp; ",  " &amp; """" &amp; F12 &amp; """" &amp; ",  " &amp; """" &amp; G12 &amp; """" &amp; ",  " &amp; """" &amp; H12 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate11",  "setVars",  "",  "",  "",  "",  "Number1=1234;Number2=11;Action=times;Answer=true;Function=IsDisplayed;CompareMode=IsDisplayed",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -3435,13 +3558,17 @@
         <v>102</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15">
+      <c r="I13" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A13 &amp; """" &amp; ",  " &amp; """" &amp; B13 &amp; """" &amp; ",  " &amp; """" &amp; C13 &amp; """" &amp; ",  " &amp; """" &amp; D13 &amp;  """" &amp;  ",  " &amp; """" &amp; E13 &amp; """" &amp; ",  " &amp; """" &amp; F13 &amp; """" &amp; ",  " &amp; """" &amp; G13 &amp; """" &amp; ",  " &amp; """" &amp; H13 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate12",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -3454,8 +3581,12 @@
       <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15">
+      <c r="I14" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A14 &amp; """" &amp; ",  " &amp; """" &amp; B14 &amp; """" &amp; ",  " &amp; """" &amp; C14 &amp; """" &amp; ",  " &amp; """" &amp; D14 &amp;  """" &amp;  ",  " &amp; """" &amp; E14 &amp; """" &amp; ",  " &amp; """" &amp; F14 &amp; """" &amp; ",  " &amp; """" &amp; G14 &amp; """" &amp; ",  " &amp; """" &amp; H14 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate13",  "setVars",  "",  "",  "",  "",  "Number1=1234;Number2=11;Action=times;Answer=35;Function=GetText;CompareMode=Contains",  "Set the proper values for test calculation"});</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -3463,13 +3594,17 @@
         <v>102</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15">
+      <c r="I15" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A15 &amp; """" &amp; ",  " &amp; """" &amp; B15 &amp; """" &amp; ",  " &amp; """" &amp; C15 &amp; """" &amp; ",  " &amp; """" &amp; D15 &amp;  """" &amp;  ",  " &amp; """" &amp; E15 &amp; """" &amp; ",  " &amp; """" &amp; F15 &amp; """" &amp; ",  " &amp; """" &amp; G15 &amp; """" &amp; ",  " &amp; """" &amp; H15 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate14",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCalculate",  "Invoke calculation with {Number1}, {Number2}, {Action}, {Answer}"});</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
@@ -3482,8 +3617,12 @@
       <c r="H16" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15">
+      <c r="I16" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A16 &amp; """" &amp; ",  " &amp; """" &amp; B16 &amp; """" &amp; ",  " &amp; """" &amp; C16 &amp; """" &amp; ",  " &amp; """" &amp; D16 &amp;  """" &amp;  ",  " &amp; """" &amp; E16 &amp; """" &amp; ",  " &amp; """" &amp; F16 &amp; """" &amp; ",  " &amp; """" &amp; G16 &amp; """" &amp; ",  " &amp; """" &amp; H16 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate15",  "takeScreenShot",  "",  "",  "",  "no",  "",  "Take a screen shot of the web page at this step"});</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="1" t="s">
         <v>143</v>
       </c>
@@ -3495,6 +3634,10 @@
       </c>
       <c r="H17" s="1" t="s">
         <v>144</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A17 &amp; """" &amp; ",  " &amp; """" &amp; B17 &amp; """" &amp; ",  " &amp; """" &amp; C17 &amp; """" &amp; ",  " &amp; """" &amp; D17 &amp;  """" &amp;  ",  " &amp; """" &amp; E17 &amp; """" &amp; ",  " &amp; """" &amp; F17 &amp; """" &amp; ",  " &amp; """" &amp; G17 &amp; """" &amp; ",  " &amp; """" &amp; H17 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Calculate16",  "generateReport",  "",  "",  "",  "",  "Description=Calculator Report",  "Generate Calculator Tests Report"});</v>
       </c>
     </row>
   </sheetData>
@@ -3569,10 +3712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3585,10 +3728,11 @@
     <col min="6" max="6" width="8.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="63.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3614,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -3633,8 +3777,12 @@
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+      <c r="I2" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate01",  "sendKeys",  "Id",  "number1",  "",  "",  "Value={Number1}",  "Enter value1 ('{Number1}') in the designated control"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -3653,8 +3801,12 @@
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
+      <c r="I3" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate02",  "sendKeys",  "Id",  "number2",  "",  "",  "Value={Number2}",  "Enter value2 ('{Number2}') in the designated control"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -3670,8 +3822,12 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+      <c r="I4" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate03",  "findElement",  "id",  "function",  "",  "",  "",  "Find the function dropdown"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -3687,8 +3843,12 @@
       <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15">
+      <c r="I5" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate04",  "click",  "Css",  "option[value='{Action}']",  "",  "",  "",  "Find and click the indicated item ('{Action}') to select"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -3704,8 +3864,12 @@
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
+      <c r="I6" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate05",  "click",  "Id",  "calculate",  "",  "",  "",  "Click the Calculate button"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -3727,8 +3891,12 @@
       <c r="H7" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+      <c r="I7" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate06",  "verifyWebElement",  "Id",  "answer",  "{Function}",  "",  "Value={Answer};CompareMode={CompareMode}",  "Find the answer control allowing 10 seconds and apply verification type: {CompareMode}, using function: {Function} verifying answer: {Answer}"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="1" t="s">
         <v>207</v>
       </c>
@@ -3737,6 +3905,10 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>208</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCalculate07",  "takeScreenShot",  "",  "",  "",  "",  "",  "Take a Screen Shot"});</v>
       </c>
     </row>
   </sheetData>
@@ -3843,10 +4015,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3856,9 +4028,10 @@
     <col min="3" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3884,7 +4057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -3899,8 +4072,12 @@
         <v>27</v>
       </c>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain01",  "createWebDriver",  "",  "",  "",  "",  "URL=http://www.compendiumdev.co.uk/selenium/find_by_playground.php",  ""});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -3917,8 +4094,12 @@
       <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain02",  "setVars",  "",  "",  "",  "",  "Hows=id,name,tagName;Values=div1,pName3,a;Function=GetAttribute;Attribute=Id;FindValue=a3;CompareMode=Equals",  "Set the proper values for test chaining finders"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -3930,13 +4111,17 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain03",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoChain",  "Invoke the finder chaining test"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -3953,8 +4138,12 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain04",  "setVars",  "",  "",  "",  "",  "Hows=id,name,tagName;Values=div1,pName9,a;Function=GetAttribute;Attribute=Id;FindValue=a9;CompareMode=Equals",  "Set the proper values for test chaining finders"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -3966,13 +4155,17 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain05",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoChain",  "Invoke the finder chaining test"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>145</v>
       </c>
@@ -3989,6 +4182,10 @@
       <c r="H7" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="I7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTChain06",  "generateReport",  "",  "",  "",  "",  "Description=Chaining Finders",  "Generate Chaining Finders Tests Report"});</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H5 H1">
@@ -4013,10 +4210,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4027,9 +4224,10 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="9" max="9" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4055,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1">
+    <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -4078,8 +4276,12 @@
       <c r="H2" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDChain01",  "verifyWebElement",  "{hows}",  "{values}",  "{Function}",  "",  "Value={FindValue};CompareMode={CompareMode};QueryParam={Attribute}",  "Find the control using chained locators and verify its property"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="4"/>
     </row>
   </sheetData>
@@ -4169,10 +4371,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="I2" sqref="I2:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4181,9 +4383,10 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="5" width="10" customWidth="1"/>
     <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="9" max="9" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4209,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -4226,8 +4429,12 @@
       <c r="H2" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders01",  "createWebDriver",  "",  "",  "",  "",  "URL=http://www.compendiumdev.co.uk/selenium/find_by_playground.php",  "Create a WebDriver for this test"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -4244,8 +4451,12 @@
       <c r="H3" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders02",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=Name;Value=#p31;Function=GetAttribute;FindValue=pName31;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -4257,13 +4468,17 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders03",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
@@ -4280,8 +4495,12 @@
       <c r="H5" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders04",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=Name;Value=*[id='p31'];Function=GetAttribute;FindValue=pName31;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -4293,13 +4512,17 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders05",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
@@ -4316,8 +4539,12 @@
       <c r="H7" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders06",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=Name;Value=[id='p31'];Function=GetAttribute;FindValue=pName31;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
@@ -4329,13 +4556,17 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders07",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -4352,8 +4583,12 @@
       <c r="H9" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders08",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=Name;Value=[id="p31"];Function=GetAttribute;FindValue=pName31;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
@@ -4365,13 +4600,17 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A10 &amp; """" &amp; ",  " &amp; """" &amp; B10 &amp; """" &amp; ",  " &amp; """" &amp; C10 &amp; """" &amp; ",  " &amp; """" &amp; D10 &amp;  """" &amp;  ",  " &amp; """" &amp; E10 &amp; """" &amp; ",  " &amp; """" &amp; F10 &amp; """" &amp; ",  " &amp; """" &amp; G10 &amp; """" &amp; ",  " &amp; """" &amp; H10 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders09",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
@@ -4388,8 +4627,12 @@
       <c r="H11" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A11 &amp; """" &amp; ",  " &amp; """" &amp; B11 &amp; """" &amp; ",  " &amp; """" &amp; C11 &amp; """" &amp; ",  " &amp; """" &amp; D11 &amp;  """" &amp;  ",  " &amp; """" &amp; E11 &amp; """" &amp; ",  " &amp; """" &amp; F11 &amp; """" &amp; ",  " &amp; """" &amp; G11 &amp; """" &amp; ",  " &amp; """" &amp; H11 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders10",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=[name="ulName1"];Function=GetAttribute;FindValue=ul1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -4401,13 +4644,17 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A12 &amp; """" &amp; ",  " &amp; """" &amp; B12 &amp; """" &amp; ",  " &amp; """" &amp; C12 &amp; """" &amp; ",  " &amp; """" &amp; D12 &amp;  """" &amp;  ",  " &amp; """" &amp; E12 &amp; """" &amp; ",  " &amp; """" &amp; F12 &amp; """" &amp; ",  " &amp; """" &amp; G12 &amp; """" &amp; ",  " &amp; """" &amp; H12 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders11",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
@@ -4424,8 +4671,12 @@
       <c r="H13" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A13 &amp; """" &amp; ",  " &amp; """" &amp; B13 &amp; """" &amp; ",  " &amp; """" &amp; C13 &amp; """" &amp; ",  " &amp; """" &amp; D13 &amp;  """" &amp;  ",  " &amp; """" &amp; E13 &amp; """" &amp; ",  " &amp; """" &amp; F13 &amp; """" &amp; ",  " &amp; """" &amp; G13 &amp; """" &amp; ",  " &amp; """" &amp; H13 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders12",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=*[name="ulName1"];Function=GetAttribute;FindValue=ul1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -4437,13 +4688,17 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A14 &amp; """" &amp; ",  " &amp; """" &amp; B14 &amp; """" &amp; ",  " &amp; """" &amp; C14 &amp; """" &amp; ",  " &amp; """" &amp; D14 &amp;  """" &amp;  ",  " &amp; """" &amp; E14 &amp; """" &amp; ",  " &amp; """" &amp; F14 &amp; """" &amp; ",  " &amp; """" &amp; G14 &amp; """" &amp; ",  " &amp; """" &amp; H14 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders13",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -4460,8 +4715,12 @@
       <c r="H15" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A15 &amp; """" &amp; ",  " &amp; """" &amp; B15 &amp; """" &amp; ",  " &amp; """" &amp; C15 &amp; """" &amp; ",  " &amp; """" &amp; D15 &amp;  """" &amp;  ",  " &amp; """" &amp; E15 &amp; """" &amp; ",  " &amp; """" &amp; F15 &amp; """" &amp; ",  " &amp; """" &amp; G15 &amp; """" &amp; ",  " &amp; """" &amp; H15 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders14",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=[name="ulName1"];Function=GetAttribute;FindValue=ul1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -4473,13 +4732,17 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A16 &amp; """" &amp; ",  " &amp; """" &amp; B16 &amp; """" &amp; ",  " &amp; """" &amp; C16 &amp; """" &amp; ",  " &amp; """" &amp; D16 &amp;  """" &amp;  ",  " &amp; """" &amp; E16 &amp; """" &amp; ",  " &amp; """" &amp; F16 &amp; """" &amp; ",  " &amp; """" &amp; G16 &amp; """" &amp; ",  " &amp; """" &amp; H16 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders15",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -4496,8 +4759,12 @@
       <c r="H17" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A17 &amp; """" &amp; ",  " &amp; """" &amp; B17 &amp; """" &amp; ",  " &amp; """" &amp; C17 &amp; """" &amp; ",  " &amp; """" &amp; D17 &amp;  """" &amp;  ",  " &amp; """" &amp; E17 &amp; """" &amp; ",  " &amp; """" &amp; F17 &amp; """" &amp; ",  " &amp; """" &amp; G17 &amp; """" &amp; ",  " &amp; """" &amp; H17 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders16",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=[name='ulName1'];Function=GetAttribute;FindValue=ul1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -4509,13 +4776,17 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A18 &amp; """" &amp; ",  " &amp; """" &amp; B18 &amp; """" &amp; ",  " &amp; """" &amp; C18 &amp; """" &amp; ",  " &amp; """" &amp; D18 &amp;  """" &amp;  ",  " &amp; """" &amp; E18 &amp; """" &amp; ",  " &amp; """" &amp; F18 &amp; """" &amp; ",  " &amp; """" &amp; G18 &amp; """" &amp; ",  " &amp; """" &amp; H18 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders17",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>148</v>
       </c>
@@ -4532,8 +4803,12 @@
       <c r="H19" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A19 &amp; """" &amp; ",  " &amp; """" &amp; B19 &amp; """" &amp; ",  " &amp; """" &amp; C19 &amp; """" &amp; ",  " &amp; """" &amp; D19 &amp;  """" &amp;  ",  " &amp; """" &amp; E19 &amp; """" &amp; ",  " &amp; """" &amp; F19 &amp; """" &amp; ",  " &amp; """" &amp; G19 &amp; """" &amp; ",  " &amp; """" &amp; H19 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders18",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=div.specialDiv;Function=GetAttribute;FindValue=div1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>149</v>
       </c>
@@ -4545,13 +4820,17 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A20 &amp; """" &amp; ",  " &amp; """" &amp; B20 &amp; """" &amp; ",  " &amp; """" &amp; C20 &amp; """" &amp; ",  " &amp; """" &amp; D20 &amp;  """" &amp;  ",  " &amp; """" &amp; E20 &amp; """" &amp; ",  " &amp; """" &amp; F20 &amp; """" &amp; ",  " &amp; """" &amp; G20 &amp; """" &amp; ",  " &amp; """" &amp; H20 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders19",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>150</v>
       </c>
@@ -4568,8 +4847,12 @@
       <c r="H21" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A21 &amp; """" &amp; ",  " &amp; """" &amp; B21 &amp; """" &amp; ",  " &amp; """" &amp; C21 &amp; """" &amp; ",  " &amp; """" &amp; D21 &amp;  """" &amp;  ",  " &amp; """" &amp; E21 &amp; """" &amp; ",  " &amp; """" &amp; F21 &amp; """" &amp; ",  " &amp; """" &amp; G21 &amp; """" &amp; ",  " &amp; """" &amp; H21 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders20",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=.specialDiv;Function=GetAttribute;FindValue=div1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>151</v>
       </c>
@@ -4581,13 +4864,17 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A22 &amp; """" &amp; ",  " &amp; """" &amp; B22 &amp; """" &amp; ",  " &amp; """" &amp; C22 &amp; """" &amp; ",  " &amp; """" &amp; D22 &amp;  """" &amp;  ",  " &amp; """" &amp; E22 &amp; """" &amp; ",  " &amp; """" &amp; F22 &amp; """" &amp; ",  " &amp; """" &amp; G22 &amp; """" &amp; ",  " &amp; """" &amp; H22 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders21",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>152</v>
       </c>
@@ -4604,8 +4891,12 @@
       <c r="H23" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A23 &amp; """" &amp; ",  " &amp; """" &amp; B23 &amp; """" &amp; ",  " &amp; """" &amp; C23 &amp; """" &amp; ",  " &amp; """" &amp; D23 &amp;  """" &amp;  ",  " &amp; """" &amp; E23 &amp; """" &amp; ",  " &amp; """" &amp; F23 &amp; """" &amp; ",  " &amp; """" &amp; G23 &amp; """" &amp; ",  " &amp; """" &amp; H23 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders22",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=.specialDiv;Function=GetAttribute;FindValue=div1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>153</v>
       </c>
@@ -4617,13 +4908,17 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A24 &amp; """" &amp; ",  " &amp; """" &amp; B24 &amp; """" &amp; ",  " &amp; """" &amp; C24 &amp; """" &amp; ",  " &amp; """" &amp; D24 &amp;  """" &amp;  ",  " &amp; """" &amp; E24 &amp; """" &amp; ",  " &amp; """" &amp; F24 &amp; """" &amp; ",  " &amp; """" &amp; G24 &amp; """" &amp; ",  " &amp; """" &amp; H24 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders23",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>154</v>
       </c>
@@ -4640,8 +4935,12 @@
       <c r="H25" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A25 &amp; """" &amp; ",  " &amp; """" &amp; B25 &amp; """" &amp; ",  " &amp; """" &amp; C25 &amp; """" &amp; ",  " &amp; """" &amp; D25 &amp;  """" &amp;  ",  " &amp; """" &amp; E25 &amp; """" &amp; ",  " &amp; """" &amp; F25 &amp; """" &amp; ",  " &amp; """" &amp; G25 &amp; """" &amp; ",  " &amp; """" &amp; H25 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders24",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=id;Value=*.specialDiv;Function=GetAttribute;FindValue=div1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>155</v>
       </c>
@@ -4653,13 +4952,17 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A26 &amp; """" &amp; ",  " &amp; """" &amp; B26 &amp; """" &amp; ",  " &amp; """" &amp; C26 &amp; """" &amp; ",  " &amp; """" &amp; D26 &amp;  """" &amp;  ",  " &amp; """" &amp; E26 &amp; """" &amp; ",  " &amp; """" &amp; F26 &amp; """" &amp; ",  " &amp; """" &amp; G26 &amp; """" &amp; ",  " &amp; """" &amp; H26 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders25",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>156</v>
       </c>
@@ -4676,8 +4979,12 @@
       <c r="H27" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A27 &amp; """" &amp; ",  " &amp; """" &amp; B27 &amp; """" &amp; ",  " &amp; """" &amp; C27 &amp; """" &amp; ",  " &amp; """" &amp; D27 &amp;  """" &amp;  ",  " &amp; """" &amp; E27 &amp; """" &amp; ",  " &amp; """" &amp; F27 &amp; """" &amp; ",  " &amp; """" &amp; G27 &amp; """" &amp; ",  " &amp; """" &amp; H27 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders26",  "setVars",  "",  "",  "",  "",  "How=Css;Attribute=name;Value=li;Function=GetAttribute;FindValue=liName1;CompareMode=Equals",  "Set the proper values for testing of css finders"});</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -4689,13 +4996,17 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A28 &amp; """" &amp; ",  " &amp; """" &amp; B28 &amp; """" &amp; ",  " &amp; """" &amp; C28 &amp; """" &amp; ",  " &amp; """" &amp; D28 &amp;  """" &amp;  ",  " &amp; """" &amp; E28 &amp; """" &amp; ",  " &amp; """" &amp; F28 &amp; """" &amp; ",  " &amp; """" &amp; G28 &amp; """" &amp; ",  " &amp; """" &amp; H28 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders27",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!DDTRoot.xlsx!DoCssFinder",  "Invoke the css finder test of this instance"});</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>158</v>
       </c>
@@ -4712,6 +5023,10 @@
       <c r="H29" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="I29" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A29 &amp; """" &amp; ",  " &amp; """" &amp; B29 &amp; """" &amp; ",  " &amp; """" &amp; C29 &amp; """" &amp; ",  " &amp; """" &amp; D29 &amp;  """" &amp;  ",  " &amp; """" &amp; E29 &amp; """" &amp; ",  " &amp; """" &amp; F29 &amp; """" &amp; ",  " &amp; """" &amp; G29 &amp; """" &amp; ",  " &amp; """" &amp; H29 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTCssFinders28",  "generateReport",  "",  "",  "",  "",  "Description=CSS Finders",  "Generate CSS Finders Tests Report"});</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 H3">
@@ -4992,10 +5307,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5006,9 +5321,10 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="9" max="9" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -5034,7 +5350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1">
+    <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -5057,8 +5373,12 @@
       <c r="H2" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCssFinder01",  "verifyWebElement",  "{how}",  "{value}",  "{Function}",  "",  "Value={FindValue};CompareMode={CompareMode};QueryParam={Attribute}",  "Find the control and verify its property "});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>201</v>
       </c>
@@ -5081,8 +5401,12 @@
       <c r="H3" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCssFinder02",  "verifyElementSize",  "{how}",  "{value}",  "getText",  "",  "Value=3;CompareMode=gt;QueryParam={Attribute};class=jaborski",  "Verify the size of the attribute is &gt; 3"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>202</v>
       </c>
@@ -5104,6 +5428,10 @@
       </c>
       <c r="H4" s="1" t="s">
         <v>204</v>
+      </c>
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DoCssFinder03",  "verifyElementSize",  "{how}",  "{value}",  "getText",  "",  "Value=3.And.2000;CompareMode=between;QueryParam={Attribute};class=jaborski",  "Verify the size of the attribute is between 3 and 50"});</v>
       </c>
     </row>
   </sheetData>
@@ -5257,10 +5585,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5271,9 +5599,10 @@
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="7" max="7" width="50.5703125" customWidth="1"/>
+    <col min="9" max="9" width="69.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -5299,7 +5628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -5316,8 +5645,12 @@
       <c r="H2" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames01",  "createWebDriver",  "",  "",  "",  "",  "URL=http://www.compendiumdev.co.uk/selenium/frames",  "Create a WebDriver for this test"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -5336,8 +5669,12 @@
       <c r="H3" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames02",  "verifyWebDriver",  "",  "",  "GetTitle",  "",  "Value=Frameset Example Title (Example 6);CompareMode=Equals",  "Verify the title of the page"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -5354,8 +5691,12 @@
       <c r="H4" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames03",  "switchToFrame",  "",  "",  "",  "",  "Value=content",  "Switch to the content frame"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -5374,8 +5715,12 @@
       <c r="H5" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames04",  "click",  "Css",  "a[href='green.html']",  "",  "",  "",  "Click the link for the green page"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -5396,8 +5741,12 @@
       <c r="H6" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames05",  "findElement",  "Css",  "h1[id='green']",  "",  "",  "WaitTime=10",  "Find the green page "});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
@@ -5416,8 +5765,12 @@
       <c r="H7" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames06",  "click",  "Css",  "a[href='content.html']",  "",  "",  "",  "Click the link for the content page"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>89</v>
       </c>
@@ -5436,8 +5789,12 @@
       <c r="H8" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames07",  "findElement",  "xpath",  "//h1[.='Content']",  "",  "",  "",  "Find the Content page again"});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>90</v>
       </c>
@@ -5460,8 +5817,12 @@
       <c r="H9" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames08",  "verifyWebElement",  "xpath",  "//h1[.='Content']",  "GetText",  "",  "Value=Content;CompareMode=Is;WaitTime=10",  "Find the Content page again"});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>161</v>
       </c>
@@ -5478,6 +5839,10 @@
       <c r="H10" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="I10" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A10 &amp; """" &amp; ",  " &amp; """" &amp; B10 &amp; """" &amp; ",  " &amp; """" &amp; C10 &amp; """" &amp; ",  " &amp; """" &amp; D10 &amp;  """" &amp;  ",  " &amp; """" &amp; E10 &amp; """" &amp; ",  " &amp; """" &amp; F10 &amp; """" &amp; ",  " &amp; """" &amp; G10 &amp; """" &amp; ",  " &amp; """" &amp; H10 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"DDTFrames09",  "generateReport",  "",  "",  "",  "",  "Description=Frame Switching",  "Generate Frame Switching Tests Report"});</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H1">
@@ -5502,10 +5867,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5515,9 +5880,10 @@
     <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
     <col min="7" max="7" width="92.140625" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -5543,7 +5909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>165</v>
       </c>
@@ -5560,8 +5926,12 @@
       <c r="H2" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify01",  "verify",  "",  "",  "",  "",  "Value=12345;ActualValue=23456;Class=Int;CompareMode=&gt;=",  "Dummy Integer test"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -5578,8 +5948,12 @@
       <c r="H3" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify02",  "verify",  "",  "",  "",  "",  "Value=-12,345;ActualValue=23,456,456,789;Class=Long;CompareMode=GT",  "Dummy Long test"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>167</v>
       </c>
@@ -5596,8 +5970,12 @@
       <c r="H4" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify03",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001;ActualValue=23,456,456,789.00007;Class=Decimal;CompareMode=!=",  "Dummy Decimal test"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -5614,8 +5992,12 @@
       <c r="H5" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify04",  "verify",  "",  "",  "",  "",  "Value=$12,345;ActualValue=$23,456;Class=Amount;CompareMode=GreaterThan",  "Dummy Currency test"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>169</v>
       </c>
@@ -5632,8 +6014,12 @@
       <c r="H6" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify05",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001;ActualValue=;Class=Decimal;CompareMode=empty",  "Dummy Decimal test"});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>170</v>
       </c>
@@ -5650,8 +6036,12 @@
       <c r="H7" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify06",  "verify",  "",  "",  "",  "",  "Value=02/03/2000;ActualValue=03/02/2010;Class=Date;CompareMode=ge;Option=MM/dd/yyyy",  "Dummy Date test"});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>171</v>
       </c>
@@ -5668,8 +6058,12 @@
       <c r="H8" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A8 &amp; """" &amp; ",  " &amp; """" &amp; B8 &amp; """" &amp; ",  " &amp; """" &amp; C8 &amp; """" &amp; ",  " &amp; """" &amp; D8 &amp;  """" &amp;  ",  " &amp; """" &amp; E8 &amp; """" &amp; ",  " &amp; """" &amp; F8 &amp; """" &amp; ",  " &amp; """" &amp; G8 &amp; """" &amp; ",  " &amp; """" &amp; H8 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify07",  "verify",  "",  "",  "",  "",  "Value=02/03/2000.and.05/05/2012;ActualValue=03/02/2010;Class=Date;CompareMode=between;Option=MM/dd/yyyy",  "Test date between early and late date"});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -5686,8 +6080,12 @@
       <c r="H9" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify08",  "verify",  "",  "",  "",  "",  "Value=-12,345.0001.and.23,456;ActualValue=100;Class=Decimal;CompareMode=Between",  "Dummy Decimal Between test"});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>192</v>
       </c>
@@ -5706,6 +6104,10 @@
       <c r="H10" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="I10" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A10 &amp; """" &amp; ",  " &amp; """" &amp; B10 &amp; """" &amp; ",  " &amp; """" &amp; C10 &amp; """" &amp; ",  " &amp; """" &amp; D10 &amp;  """" &amp;  ",  " &amp; """" &amp; E10 &amp; """" &amp; ",  " &amp; """" &amp; F10 &amp; """" &amp; ",  " &amp; """" &amp; G10 &amp; """" &amp; ",  " &amp; """" &amp; H10 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Verify09",  "generateReport",  "",  "",  "",  "no",  "Description=Dummy Tests Should Pass;EmailBody=This test should pass",  "Generate Dummy Tests Report (Pass)"});</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H4 H1 H6:H9">

</xml_diff>

<commit_message>
Most recent 1.2.1 changes - Resolve Issue With FireFox above 1.25.01 & Selenium
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="195">
   <si>
     <t>Action</t>
   </si>
@@ -1925,7 +1925,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1985,9 +1985,6 @@
       <c r="B3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G3" s="1" t="s">
         <v>175</v>
       </c>
@@ -2052,9 +2049,6 @@
       </c>
       <c r="B7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Versuib 1.2.2 - Bug fixes and new features
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="465" windowWidth="26220" windowHeight="10815" tabRatio="714"/>
+    <workbookView xWindow="210" yWindow="60" windowWidth="22755" windowHeight="9465" tabRatio="714"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="198">
   <si>
     <t>Action</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Click the link for the green page</t>
   </si>
   <si>
-    <t>switchToFrame</t>
-  </si>
-  <si>
     <t xml:space="preserve">Find the green page </t>
   </si>
   <si>
@@ -609,6 +606,18 @@
   </si>
   <si>
     <t>Verify the size of the attribute is between 3 and 2000</t>
+  </si>
+  <si>
+    <t>waitUntil</t>
+  </si>
+  <si>
+    <t>Value={Answer};CompareMode={CompareMode};TotalWaitTime=10</t>
+  </si>
+  <si>
+    <t>Try Wait Until</t>
+  </si>
+  <si>
+    <t>switchTo</t>
   </si>
 </sst>
 </file>
@@ -701,127 +710,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="108">
     <dxf>
       <font>
         <b/>
@@ -1925,7 +1814,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1949,13 +1838,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1969,24 +1858,30 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>27</v>
@@ -1994,16 +1889,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>28</v>
@@ -2011,16 +1906,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>29</v>
@@ -2028,77 +1923,77 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="123" priority="38" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="39" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="120" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2133,13 +2028,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2153,218 +2048,218 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2421,65 +2316,65 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2517,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2537,13 +2432,13 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -2551,7 +2446,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2565,30 +2460,30 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>16</v>
@@ -2596,13 +2491,13 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -2610,13 +2505,13 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>16</v>
@@ -2624,13 +2519,13 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>13</v>
@@ -2638,13 +2533,13 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>16</v>
@@ -2652,13 +2547,13 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>13</v>
@@ -2666,13 +2561,13 @@
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
@@ -2680,13 +2575,13 @@
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
@@ -2694,13 +2589,13 @@
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>16</v>
@@ -2708,13 +2603,13 @@
     </row>
     <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>13</v>
@@ -2722,13 +2617,13 @@
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>16</v>
@@ -2736,13 +2631,13 @@
     </row>
     <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
@@ -2750,7 +2645,7 @@
     </row>
     <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -2761,48 +2656,48 @@
     </row>
     <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="119" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="116" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="115" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="112" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2813,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2838,13 +2733,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2858,7 +2753,7 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -2867,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -2878,7 +2773,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2887,7 +2782,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>15</v>
@@ -2898,16 +2793,16 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
@@ -2915,16 +2810,16 @@
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>20</v>
@@ -2932,7 +2827,7 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -2941,7 +2836,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>12</v>
@@ -2949,7 +2844,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -2958,126 +2853,85 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
+      <c r="A9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>117</v>
+      <c r="F9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="111" priority="41" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="44" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="108" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="107" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="104" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="103" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="100" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="99" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="96" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="95" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="92" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="91" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="88" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H1:H4">
+    <cfRule type="cellIs" dxfId="95" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="44" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H4">
+    <cfRule type="cellIs" dxfId="92" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H8">
+    <cfRule type="cellIs" dxfId="91" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H8">
+    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3111,13 +2965,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3131,7 +2985,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3147,7 +3001,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -3157,7 +3011,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
@@ -3165,17 +3019,17 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -3183,7 +3037,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3193,7 +3047,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>25</v>
@@ -3201,17 +3055,17 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>26</v>
@@ -3219,20 +3073,20 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3282,13 +3136,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3308,20 +3162,20 @@
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3436,13 +3290,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3456,7 +3310,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3466,7 +3320,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
@@ -3474,23 +3328,23 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -3501,12 +3355,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3516,7 +3370,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -3524,17 +3378,17 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -3542,7 +3396,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -3552,7 +3406,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -3560,17 +3414,17 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>33</v>
@@ -3578,7 +3432,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -3588,7 +3442,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
@@ -3596,17 +3450,17 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -3614,7 +3468,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -3624,7 +3478,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -3632,17 +3486,17 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>33</v>
@@ -3650,7 +3504,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -3660,7 +3514,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
@@ -3668,17 +3522,17 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -3686,7 +3540,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -3696,7 +3550,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
@@ -3704,17 +3558,17 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>33</v>
@@ -3722,7 +3576,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -3732,7 +3586,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -3740,17 +3594,17 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>33</v>
@@ -3758,7 +3612,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -3768,7 +3622,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -3776,17 +3630,17 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>33</v>
@@ -3794,7 +3648,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -3804,7 +3658,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>32</v>
@@ -3812,17 +3666,17 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3830,7 +3684,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -3840,7 +3694,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
@@ -3848,17 +3702,17 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -3866,7 +3720,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -3876,7 +3730,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>32</v>
@@ -3884,17 +3738,17 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>33</v>
@@ -3902,7 +3756,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -3912,7 +3766,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -3920,17 +3774,17 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>33</v>
@@ -3938,7 +3792,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -3948,7 +3802,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>32</v>
@@ -3956,17 +3810,17 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>33</v>
@@ -3974,20 +3828,20 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -4035,13 +3889,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -4055,23 +3909,23 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
@@ -4079,50 +3933,50 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4279,7 +4133,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4300,13 +4154,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -4320,7 +4174,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -4338,7 +4192,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
@@ -4346,11 +4200,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>39</v>
@@ -4358,10 +4212,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4376,16 +4230,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4396,106 +4250,106 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -4544,13 +4398,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -4564,164 +4418,164 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More debugging, code maintenance & documentation updates
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -19,12 +19,12 @@
     <sheet name="Dummy Tests Errors" sheetId="40" r:id="rId10"/>
     <sheet name="ReadMe" sheetId="32" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="200">
   <si>
     <t>Action</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Generate Dummy Tests Report (Pass)</t>
   </si>
   <si>
-    <t>Description=Summary Report</t>
-  </si>
-  <si>
     <t>Description=Calculator Report</t>
   </si>
   <si>
@@ -618,6 +615,15 @@
   </si>
   <si>
     <t>switchTo</t>
+  </si>
+  <si>
+    <t>DDT Tests Passed</t>
+  </si>
+  <si>
+    <t>Title='Passed Report'</t>
+  </si>
+  <si>
+    <t>Title=Summary Report &amp; 'that's It</t>
   </si>
 </sst>
 </file>
@@ -1811,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1858,30 +1864,30 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>27</v>
@@ -1889,16 +1895,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>28</v>
@@ -1906,16 +1912,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>29</v>
@@ -1923,13 +1929,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>72</v>
@@ -1937,16 +1946,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>73</v>
@@ -1954,46 +1960,60 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>99</v>
+      <c r="G10" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="107" priority="38" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="39" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="104" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2048,17 +2068,17 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>74</v>
@@ -2066,17 +2086,17 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>75</v>
@@ -2084,17 +2104,17 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>76</v>
@@ -2102,17 +2122,17 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>77</v>
@@ -2120,17 +2140,17 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>76</v>
@@ -2138,17 +2158,17 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>79</v>
@@ -2156,97 +2176,97 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>78</v>
@@ -2256,7 +2276,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>80</v>
@@ -2264,34 +2284,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H4 H1 H6:H12">
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4 H1 H6:H12">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H12">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H12">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2316,65 +2336,65 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2432,13 +2452,13 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -2446,7 +2466,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2460,30 +2480,30 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>16</v>
@@ -2491,13 +2511,13 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -2505,13 +2525,13 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>16</v>
@@ -2519,13 +2539,13 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>13</v>
@@ -2533,13 +2553,13 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>16</v>
@@ -2547,13 +2567,13 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>13</v>
@@ -2561,13 +2581,13 @@
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
@@ -2575,13 +2595,13 @@
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
@@ -2589,13 +2609,13 @@
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>16</v>
@@ -2603,13 +2623,13 @@
     </row>
     <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>13</v>
@@ -2617,13 +2637,13 @@
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>16</v>
@@ -2631,13 +2651,13 @@
     </row>
     <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
@@ -2645,7 +2665,7 @@
     </row>
     <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -2656,48 +2676,48 @@
     </row>
     <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="103" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="100" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="99" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="96" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2753,7 +2773,7 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -2773,7 +2793,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2793,7 +2813,7 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -2810,7 +2830,7 @@
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -2827,7 +2847,7 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -2844,7 +2864,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -2859,7 +2879,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>48</v>
@@ -2867,10 +2887,10 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -2882,56 +2902,56 @@
         <v>60</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H4">
-    <cfRule type="cellIs" dxfId="95" priority="41" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H4">
-    <cfRule type="cellIs" dxfId="92" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H8">
-    <cfRule type="cellIs" dxfId="91" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H8">
-    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2985,7 +3005,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3001,7 +3021,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -3011,7 +3031,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
@@ -3019,7 +3039,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
@@ -3029,7 +3049,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -3037,7 +3057,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3047,7 +3067,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>25</v>
@@ -3055,7 +3075,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
@@ -3065,7 +3085,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>26</v>
@@ -3073,7 +3093,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -3083,26 +3103,26 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="87" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="84" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3172,7 +3192,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>46</v>
@@ -3183,82 +3203,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="83" priority="29" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="29" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="80" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="79" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="76" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="75" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="72" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="71" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="68" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="67" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="64" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3310,7 +3330,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3320,7 +3340,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
@@ -3328,23 +3348,23 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -3355,12 +3375,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3370,7 +3390,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -3378,7 +3398,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
@@ -3388,7 +3408,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -3396,7 +3416,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -3406,7 +3426,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -3414,7 +3434,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
@@ -3424,7 +3444,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>33</v>
@@ -3432,7 +3452,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -3442,7 +3462,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
@@ -3450,7 +3470,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
@@ -3460,7 +3480,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -3468,7 +3488,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -3478,7 +3498,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -3486,7 +3506,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
@@ -3496,7 +3516,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>33</v>
@@ -3504,7 +3524,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -3514,7 +3534,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
@@ -3522,7 +3542,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>45</v>
@@ -3532,7 +3552,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -3540,7 +3560,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -3550,7 +3570,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
@@ -3558,7 +3578,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
@@ -3568,7 +3588,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>33</v>
@@ -3576,7 +3596,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -3586,7 +3606,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -3594,7 +3614,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>45</v>
@@ -3604,7 +3624,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>33</v>
@@ -3612,7 +3632,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -3622,7 +3642,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -3630,7 +3650,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
@@ -3640,7 +3660,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>33</v>
@@ -3648,7 +3668,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -3658,7 +3678,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>32</v>
@@ -3666,7 +3686,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>45</v>
@@ -3676,7 +3696,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3684,7 +3704,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -3694,7 +3714,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
@@ -3702,7 +3722,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>45</v>
@@ -3712,7 +3732,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -3720,7 +3740,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -3730,7 +3750,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>32</v>
@@ -3738,7 +3758,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>45</v>
@@ -3748,7 +3768,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>33</v>
@@ -3756,7 +3776,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -3766,7 +3786,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -3774,7 +3794,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
@@ -3784,7 +3804,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>33</v>
@@ -3792,7 +3812,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -3802,7 +3822,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>32</v>
@@ -3810,7 +3830,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
@@ -3820,7 +3840,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>33</v>
@@ -3828,7 +3848,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>78</v>
@@ -3838,26 +3858,26 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H7 H9 H11 H13 H15 H17 H19 H21 H23 H25 H27 H29 H5 H1">
-    <cfRule type="cellIs" dxfId="63" priority="74" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="75" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="74" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="75" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="76" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7 H9 H11 H13 H15 H17 H19 H21 H23 H25 H27 H29 H5 H1">
-    <cfRule type="cellIs" dxfId="60" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="73" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3909,7 +3929,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -3925,7 +3945,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
@@ -3933,10 +3953,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>64</v>
@@ -3945,22 +3965,22 @@
         <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>64</v>
@@ -3969,158 +3989,158 @@
         <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="59" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="56" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="55" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="52" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="51" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="48" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="47" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="44" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="43" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="40" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="39" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="36" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="32" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4174,7 +4194,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -4192,7 +4212,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
@@ -4204,7 +4224,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>39</v>
@@ -4212,10 +4232,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4230,7 +4250,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -4250,7 +4270,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -4272,7 +4292,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -4292,7 +4312,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -4312,7 +4332,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -4328,7 +4348,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>44</v>
@@ -4336,7 +4356,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -4346,26 +4366,26 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="23" priority="78" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="79" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="78" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="79" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="80" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="20" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="77" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4418,17 +4438,17 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>74</v>
@@ -4436,17 +4456,17 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>75</v>
@@ -4454,17 +4474,17 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>76</v>
@@ -4472,17 +4492,17 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>77</v>
@@ -4490,17 +4510,17 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>76</v>
@@ -4508,17 +4528,17 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>79</v>
@@ -4526,43 +4546,43 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -4572,7 +4592,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>81</v>
@@ -4580,50 +4600,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H4 H1 H6:H9">
-    <cfRule type="cellIs" dxfId="19" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4 H1 H6:H9">
-    <cfRule type="cellIs" dxfId="16" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Various bugs, Extent Reports Improvements
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="60" windowWidth="22755" windowHeight="9465" tabRatio="714"/>
+    <workbookView xWindow="210" yWindow="60" windowWidth="22755" windowHeight="9465" tabRatio="714" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Dummy Tests Errors" sheetId="40" r:id="rId10"/>
     <sheet name="ReadMe" sheetId="32" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="197">
   <si>
     <t>Action</t>
   </si>
@@ -398,12 +398,6 @@
     <t>Value={Answer};CompareMode={CompareMode}</t>
   </si>
   <si>
-    <t>Hows=id,name,tagName;Values=div1,pName3,a;Function=GetAttribute;Attribute=Id;FindValue=a3;CompareMode=Equals</t>
-  </si>
-  <si>
-    <t>Hows=id,name,tagName;Values=div1,pName9,a;Function=GetAttribute;Attribute=Id;FindValue=a9;CompareMode=Equals</t>
-  </si>
-  <si>
     <t>Value={FindValue};CompareMode={CompareMode};QueryParam={Attribute}</t>
   </si>
   <si>
@@ -461,9 +455,6 @@
     <t>Value=-12,345.0001;ActualValue=23,456,456,789.00007;Class=Decimal;CompareMode=!=</t>
   </si>
   <si>
-    <t>Value=$12,345;ActualValue=$23,456;Class=Amount;CompareMode=GreaterThan</t>
-  </si>
-  <si>
     <t>Value=-12,345.0001;ActualValue=;Class=Decimal;CompareMode=empty</t>
   </si>
   <si>
@@ -605,15 +596,6 @@
     <t>Verify the size of the attribute is between 3 and 2000</t>
   </si>
   <si>
-    <t>waitUntil</t>
-  </si>
-  <si>
-    <t>Value={Answer};CompareMode={CompareMode};TotalWaitTime=10</t>
-  </si>
-  <si>
-    <t>Try Wait Until</t>
-  </si>
-  <si>
     <t>switchTo</t>
   </si>
   <si>
@@ -624,6 +606,15 @@
   </si>
   <si>
     <t>Title=Summary Report &amp; 'that's It</t>
+  </si>
+  <si>
+    <t>Value=$12,345;ActualValue=$23,456;Class=Currency;CompareMode=GreaterThan</t>
+  </si>
+  <si>
+    <t>Hows=id`name`tagName;Values=div1`pName3`a;Function=GetAttribute;Attribute=Id;FindValue=a3;CompareMode=Equals</t>
+  </si>
+  <si>
+    <t>Hows=id`name`tagName;Values=div1`pName9`a;Function=GetAttribute;Attribute=Id;FindValue=a9;CompareMode=Equals</t>
   </si>
 </sst>
 </file>
@@ -716,37 +707,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="104">
     <dxf>
       <font>
         <b/>
@@ -1819,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1864,30 +1825,24 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>27</v>
@@ -1895,16 +1850,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>28</v>
@@ -1912,16 +1864,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>29</v>
@@ -1929,16 +1878,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>72</v>
@@ -1946,13 +1892,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>73</v>
@@ -1960,41 +1906,41 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>98</v>
@@ -2002,18 +1948,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="3" priority="38" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="39" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H5">
-    <cfRule type="cellIs" dxfId="0" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2027,7 +1973,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2068,7 +2014,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>89</v>
@@ -2078,7 +2024,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>74</v>
@@ -2086,7 +2032,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>89</v>
@@ -2096,7 +2042,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>75</v>
@@ -2104,7 +2050,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -2114,7 +2060,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>76</v>
@@ -2122,7 +2068,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>89</v>
@@ -2132,7 +2078,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>77</v>
@@ -2140,7 +2086,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>89</v>
@@ -2150,7 +2096,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>76</v>
@@ -2158,7 +2104,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>89</v>
@@ -2168,7 +2114,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>79</v>
@@ -2176,7 +2122,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>89</v>
@@ -2186,7 +2132,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>100</v>
@@ -2194,7 +2140,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>89</v>
@@ -2204,7 +2150,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>101</v>
@@ -2212,7 +2158,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>89</v>
@@ -2222,7 +2168,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>102</v>
@@ -2230,7 +2176,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>89</v>
@@ -2240,7 +2186,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>103</v>
@@ -2248,7 +2194,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>89</v>
@@ -2258,7 +2204,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>104</v>
@@ -2266,7 +2212,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>78</v>
@@ -2274,9 +2220,11 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>80</v>
@@ -2408,7 +2356,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2452,7 +2400,7 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -2466,7 +2414,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2480,24 +2428,24 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -2511,13 +2459,13 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -2525,7 +2473,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -2539,13 +2487,13 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>13</v>
@@ -2553,7 +2501,7 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -2567,13 +2515,13 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>13</v>
@@ -2581,7 +2529,7 @@
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -2595,13 +2543,13 @@
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
@@ -2609,7 +2557,7 @@
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -2623,13 +2571,13 @@
     </row>
     <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>13</v>
@@ -2637,7 +2585,7 @@
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -2651,13 +2599,13 @@
     </row>
     <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
@@ -2665,7 +2613,7 @@
     </row>
     <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -2676,48 +2624,51 @@
     </row>
     <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>82</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="107" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H16">
-    <cfRule type="cellIs" dxfId="104" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="103" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="100" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2728,10 +2679,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2773,7 +2724,7 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -2793,7 +2744,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2813,7 +2764,7 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -2830,7 +2781,7 @@
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -2847,7 +2798,7 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -2864,7 +2815,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -2887,71 +2838,32 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>194</v>
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15">
-      <c r="A9" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="1" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H4">
-    <cfRule type="cellIs" dxfId="99" priority="41" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="44" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H4">
-    <cfRule type="cellIs" dxfId="96" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H8">
-    <cfRule type="cellIs" dxfId="95" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H8">
-    <cfRule type="cellIs" dxfId="92" priority="10" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H1:H7">
+    <cfRule type="cellIs" dxfId="3" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="44" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H7">
+    <cfRule type="cellIs" dxfId="0" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2965,7 +2877,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3005,7 +2917,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3021,7 +2933,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -3031,7 +2943,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
@@ -3039,7 +2951,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
@@ -3049,7 +2961,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -3057,7 +2969,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3067,7 +2979,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>25</v>
@@ -3075,7 +2987,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
@@ -3085,7 +2997,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>26</v>
@@ -3093,7 +3005,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -3101,7 +3013,9 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>83</v>
       </c>
@@ -3192,7 +3106,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>46</v>
@@ -3290,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3330,7 +3244,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -3340,7 +3254,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
@@ -3348,23 +3262,23 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -3375,12 +3289,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3390,7 +3304,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -3398,7 +3312,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
@@ -3408,7 +3322,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -3416,7 +3330,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -3426,7 +3340,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -3434,7 +3348,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
@@ -3444,7 +3358,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>33</v>
@@ -3452,7 +3366,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -3462,7 +3376,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
@@ -3470,7 +3384,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
@@ -3480,7 +3394,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -3488,7 +3402,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -3498,7 +3412,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -3506,7 +3420,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
@@ -3516,7 +3430,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>33</v>
@@ -3524,7 +3438,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -3534,7 +3448,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
@@ -3542,7 +3456,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>45</v>
@@ -3552,7 +3466,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -3560,7 +3474,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -3570,7 +3484,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
@@ -3578,7 +3492,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
@@ -3588,7 +3502,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>33</v>
@@ -3596,7 +3510,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -3606,7 +3520,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -3614,7 +3528,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>45</v>
@@ -3624,7 +3538,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>33</v>
@@ -3632,7 +3546,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -3642,7 +3556,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -3650,7 +3564,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
@@ -3660,7 +3574,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>33</v>
@@ -3668,7 +3582,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -3678,7 +3592,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>32</v>
@@ -3686,7 +3600,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>45</v>
@@ -3696,7 +3610,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3704,7 +3618,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -3714,7 +3628,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
@@ -3722,7 +3636,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>45</v>
@@ -3732,7 +3646,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -3740,7 +3654,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -3750,7 +3664,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>32</v>
@@ -3758,7 +3672,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>45</v>
@@ -3768,7 +3682,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>33</v>
@@ -3776,7 +3690,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -3786,7 +3700,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -3794,7 +3708,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
@@ -3804,7 +3718,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>33</v>
@@ -3812,7 +3726,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -3822,7 +3736,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>32</v>
@@ -3830,7 +3744,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
@@ -3840,7 +3754,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>33</v>
@@ -3848,7 +3762,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>78</v>
@@ -3856,7 +3770,9 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>85</v>
       </c>
@@ -3929,7 +3845,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -3945,7 +3861,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
@@ -3953,7 +3869,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>113</v>
@@ -3969,7 +3885,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>112</v>
@@ -3977,7 +3893,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>113</v>
@@ -3993,10 +3909,10 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4153,7 +4069,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4194,7 +4110,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -4212,7 +4128,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
@@ -4224,7 +4140,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>39</v>
@@ -4232,10 +4148,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4250,7 +4166,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -4270,7 +4186,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -4292,7 +4208,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -4312,7 +4228,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -4332,7 +4248,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -4348,7 +4264,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>44</v>
@@ -4356,7 +4272,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -4364,7 +4280,9 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>87</v>
       </c>
@@ -4398,7 +4316,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4438,7 +4356,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>89</v>
@@ -4448,7 +4366,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>74</v>
@@ -4456,7 +4374,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>89</v>
@@ -4466,7 +4384,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>75</v>
@@ -4474,7 +4392,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -4484,7 +4402,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>76</v>
@@ -4492,7 +4410,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>89</v>
@@ -4502,7 +4420,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>77</v>
@@ -4510,7 +4428,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>89</v>
@@ -4520,7 +4438,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>76</v>
@@ -4528,7 +4446,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>89</v>
@@ -4538,7 +4456,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>79</v>
@@ -4546,7 +4464,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>89</v>
@@ -4556,7 +4474,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>100</v>
@@ -4564,7 +4482,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>89</v>
@@ -4574,7 +4492,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>101</v>
@@ -4582,7 +4500,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -4590,9 +4508,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Renamed Data attribute to Params
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="60" windowWidth="22755" windowHeight="9465" tabRatio="714" activeTab="2"/>
+    <workbookView xWindow="210" yWindow="60" windowWidth="22755" windowHeight="9450" tabRatio="714" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>Set the Browser and Base URL - TODO: Resolve issue with Browser Type</t>
   </si>
   <si>
@@ -615,6 +612,9 @@
   </si>
   <si>
     <t>Hows=id`name`tagName;Values=div1`pName9`a;Function=GetAttribute;Attribute=Id;FindValue=a9;CompareMode=Equals</t>
+  </si>
+  <si>
+    <t>Params</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1781,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1799,25 +1799,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -1825,125 +1825,125 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1988,25 +1988,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2014,252 +2014,252 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H4 H1 H6:H12">
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4 H1 H6:H12">
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H12">
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H12">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2271,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2284,65 +2284,65 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2356,7 +2356,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2374,25 +2374,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2400,243 +2400,243 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2681,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2704,19 +2704,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2724,146 +2724,146 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H7">
-    <cfRule type="cellIs" dxfId="3" priority="41" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H7">
-    <cfRule type="cellIs" dxfId="0" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2877,7 +2877,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2891,25 +2891,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2917,126 +2917,126 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="91" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="88" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3049,7 +3049,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,25 +3064,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -3090,26 +3090,26 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3117,82 +3117,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="87" priority="29" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="29" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="84" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="83" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="80" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="79" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="76" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="75" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="72" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="71" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="68" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3204,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3218,25 +3218,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -3244,44 +3244,44 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3289,511 +3289,511 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H7 H9 H11 H13 H15 H17 H19 H21 H23 H25 H27 H29 H5 H1">
-    <cfRule type="cellIs" dxfId="67" priority="74" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="75" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="74" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="75" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="76" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7 H9 H11 H13 H15 H17 H19 H21 H23 H25 H27 H29 H5 H1">
-    <cfRule type="cellIs" dxfId="64" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="73" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3805,7 +3805,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3819,25 +3821,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -3845,218 +3847,218 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="63" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="60" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="59" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="56" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="55" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="52" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="51" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="48" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="44" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="43" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="40" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="35" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="31" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4069,7 +4071,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4084,25 +4086,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -4110,200 +4112,200 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="27" priority="78" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="79" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="78" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="79" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="80" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="24" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="77" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4316,7 +4318,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4330,25 +4332,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -4356,214 +4358,214 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H4 H1 H6:H9">
-    <cfRule type="cellIs" dxfId="23" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4 H1 H6:H9">
-    <cfRule type="cellIs" dxfId="20" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="19" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Introduce DragAndDrop verb and other minor changes
</commit_message>
<xml_diff>
--- a/Data/DDTRoot.xlsx
+++ b/Data/DDTRoot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="270" yWindow="690" windowWidth="24240" windowHeight="8805" tabRatio="714" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="270" yWindow="690" windowWidth="24240" windowHeight="8805" tabRatio="714" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -30,18 +30,19 @@
     <sheet name="CalcTests" sheetId="45" r:id="rId16"/>
     <sheet name="Divide999By333" sheetId="46" r:id="rId17"/>
     <sheet name="Multiply3By3By3" sheetId="47" r:id="rId18"/>
-    <sheet name="ReadMe" sheetId="32" r:id="rId19"/>
-    <sheet name="Help" sheetId="50" r:id="rId20"/>
+    <sheet name="DragAndDrop" sheetId="51" r:id="rId19"/>
+    <sheet name="ReadMe" sheetId="32" r:id="rId20"/>
+    <sheet name="Help" sheetId="50" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="Verbs">Help!$A$2:$A$35</definedName>
+    <definedName name="Verbs">Help!$A$2:$A$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="448">
   <si>
     <t>Action</t>
   </si>
@@ -721,9 +722,6 @@
     <t>scpt0</t>
   </si>
   <si>
-    <t>url=https://www.google.com/#q=calculator;BaseTitle=calculator - Google Search</t>
-  </si>
-  <si>
     <t>Set the Browser and Base URL - calculator - Google Search</t>
   </si>
   <si>
@@ -925,9 +923,6 @@
     <t>Title=Dummy Tests With Errors;EmailBody=This test should FAIL big time</t>
   </si>
   <si>
-    <t>Title=Summary Report</t>
-  </si>
-  <si>
     <t>Title=Calculator Report</t>
   </si>
   <si>
@@ -1307,6 +1302,90 @@
   </si>
   <si>
     <t>Hover over the (inner) Input / Answer element</t>
+  </si>
+  <si>
+    <t>Click the "More" item</t>
+  </si>
+  <si>
+    <t>Click the "images" element</t>
+  </si>
+  <si>
+    <t>dragAndDrop</t>
+  </si>
+  <si>
+    <t>DragAndDrop</t>
+  </si>
+  <si>
+    <t>Drag and Drop (must specify two locType and locSpecs using a separator)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drag an image and drop it </t>
+  </si>
+  <si>
+    <t>InputSpecs=File!DDTRoot.xlsx!DragAndDrop</t>
+  </si>
+  <si>
+    <t>Drag and Drop Test</t>
+  </si>
+  <si>
+    <t>//*[@id="_P9o"]/g-menu-item[1]/div</t>
+  </si>
+  <si>
+    <t>//*[@id="hdtb-msb"]/div[1]/g-dropdown-menu/g-popup/div[1]/a</t>
+  </si>
+  <si>
+    <t>ResizePage</t>
+  </si>
+  <si>
+    <t>Resize the current WebPage to x, y dimension</t>
+  </si>
+  <si>
+    <t>URL={url};ptp=QSOF</t>
+  </si>
+  <si>
+    <t>url=http://www.w3schools.com/html/html5_draganddrop.asp</t>
+  </si>
+  <si>
+    <t>id;id</t>
+  </si>
+  <si>
+    <t>drag1;div2</t>
+  </si>
+  <si>
+    <t>Title=Summary Report;isFinal=true</t>
+  </si>
+  <si>
+    <t>Find the 'to' element</t>
+  </si>
+  <si>
+    <t>Find the 'from' element</t>
+  </si>
+  <si>
+    <t>//*[@id="drag1"]</t>
+  </si>
+  <si>
+    <t>//*[@id="div2"]</t>
+  </si>
+  <si>
+    <t>WaitTime=2</t>
+  </si>
+  <si>
+    <t>//*[@id="main"]/h1/span</t>
+  </si>
+  <si>
+    <t>Find the page title span</t>
+  </si>
+  <si>
+    <t>url=https://www.google.com/#q=google+calculator</t>
+  </si>
+  <si>
+    <t>url=https://www.google.com/search?q=google+calculator</t>
+  </si>
+  <si>
+    <t>WaitTime=15</t>
+  </si>
+  <si>
+    <t>Wait for 15 seconds…</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1432,11 +1511,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1463,11 +1551,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="304">
+  <dxfs count="308">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4085,7 +4204,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4135,10 +4254,10 @@
         <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4155,7 +4274,7 @@
         <v>220</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4251,42 +4370,42 @@
         <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>294</v>
+        <v>436</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 H3:H6">
-    <cfRule type="cellIs" dxfId="303" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="302" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="301" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="306" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="305" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H3:H6">
-    <cfRule type="cellIs" dxfId="300" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="299" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="298" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="297" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="302" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="301" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="296" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4578,7 +4697,7 @@
         <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>71</v>
@@ -4586,18 +4705,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="83" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="80" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4777,50 +4896,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="79" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="76" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="75" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="72" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="71" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="68" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5050,50 +5169,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="67" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="64" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="63" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="60" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="59" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5109,10 +5228,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5150,7 +5269,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -5160,15 +5279,15 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>44</v>
@@ -5176,17 +5295,19 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>44</v>
@@ -5194,124 +5315,140 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>304</v>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="H5" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="55" priority="25" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="25" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="52" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="51" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="48" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="44" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="40" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="32" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="31" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5326,17 +5463,17 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="79.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5368,7 +5505,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -5378,15 +5515,15 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -5396,63 +5533,74 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>432</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="H4" t="s">
+        <v>447</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="27" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="24" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="23" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="20" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B69">
       <formula1>Verbs</formula1>
     </dataValidation>
   </dataValidations>
@@ -5464,7 +5612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -5511,25 +5659,25 @@
         <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5541,25 +5689,25 @@
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5571,25 +5719,25 @@
         <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5601,25 +5749,25 @@
         <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5631,25 +5779,25 @@
         <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5661,25 +5809,25 @@
         <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5691,25 +5839,25 @@
         <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5721,25 +5869,25 @@
         <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5751,25 +5899,25 @@
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5781,25 +5929,25 @@
         <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5811,25 +5959,25 @@
         <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5841,25 +5989,25 @@
         <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5871,25 +6019,25 @@
         <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5901,25 +6049,25 @@
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5931,25 +6079,25 @@
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5961,25 +6109,25 @@
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5991,25 +6139,25 @@
         <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -6021,25 +6169,25 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H37" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -6051,25 +6199,25 @@
         <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6081,25 +6229,25 @@
         <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -6111,25 +6259,25 @@
         <v>54</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6141,41 +6289,41 @@
         <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6193,7 +6341,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B70"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6233,7 +6381,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -6241,15 +6389,15 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>44</v>
@@ -6257,31 +6405,31 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B69">
       <formula1>Verbs</formula1>
     </dataValidation>
   </dataValidations>
@@ -6341,10 +6489,10 @@
         <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6356,10 +6504,10 @@
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6371,10 +6519,10 @@
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6386,17 +6534,17 @@
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6408,29 +6556,29 @@
         <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6442,10 +6590,10 @@
         <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6457,10 +6605,10 @@
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6472,10 +6620,10 @@
         <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6487,17 +6635,17 @@
         <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6509,10 +6657,10 @@
         <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6524,33 +6672,33 @@
         <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6615,10 +6763,10 @@
         <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6630,10 +6778,10 @@
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6645,10 +6793,10 @@
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6660,10 +6808,10 @@
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6675,10 +6823,10 @@
         <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6690,17 +6838,17 @@
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6712,10 +6860,10 @@
         <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6727,33 +6875,33 @@
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6771,138 +6919,223 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="121" style="11" customWidth="1"/>
-    <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>404</v>
-      </c>
-      <c r="B6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>405</v>
-      </c>
-      <c r="B7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>81</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="H4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="H5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="H8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="H9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="H10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H11" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H3">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H3">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:B74">
+      <formula1>TheVerbs</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B71 B3:B5">
+      <formula1>Verbs</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6910,7 +7143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -7170,7 +7403,7 @@
         <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>73</v>
@@ -7178,66 +7411,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H15">
-    <cfRule type="cellIs" dxfId="295" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="294" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="293" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="298" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="297" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H15">
-    <cfRule type="cellIs" dxfId="292" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="291" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="290" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="294" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="288" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="287" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="286" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="285" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="290" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="284" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="283" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="282" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="286" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="280" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7256,10 +7489,147 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="121" style="11" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="B7" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7270,7 +7640,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -7278,274 +7648,290 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B11" s="8" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B16" s="10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="B14" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>349</v>
+        <v>430</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>383</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -7730,98 +8116,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="279" priority="41" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="278" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="282" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="276" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="275" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="278" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="277" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="272" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="271" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="270" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="274" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="273" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="268" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="267" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="264" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="263" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="261" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="266" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="265" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="260" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="259" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="258" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="262" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="256" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7983,7 +8369,7 @@
         <v>82</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>74</v>
@@ -7991,18 +8377,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="255" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="258" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="257" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H5 H1">
-    <cfRule type="cellIs" dxfId="252" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8085,82 +8471,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="251" priority="29" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="249" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="29" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="254" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="248" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="247" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="250" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="249" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="244" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="243" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="240" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="239" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="242" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="241" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="236" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="235" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="238" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="237" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="232" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8718,7 +9104,7 @@
         <v>82</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>75</v>
@@ -8737,274 +9123,274 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 H3">
-    <cfRule type="cellIs" dxfId="231" priority="74" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="75" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="74" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="75" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="76" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H3">
-    <cfRule type="cellIs" dxfId="228" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="73" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="227" priority="62" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="63" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="64" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="62" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="230" priority="63" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="229" priority="64" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="224" priority="61" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="61" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="223" priority="58" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="58" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="220" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="219" priority="54" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="55" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="54" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="222" priority="55" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="216" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="215" priority="50" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="51" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="50" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="51" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="52" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="212" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="49" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="211" priority="46" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="47" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="46" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="47" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="48" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="208" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="45" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="207" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="209" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="204" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="203" priority="38" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="39" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="200" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="199" priority="34" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="35" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="34" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="35" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="196" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="195" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="197" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="192" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="191" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="188" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="187" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="189" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="184" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="183" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="180" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="179" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="176" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="175" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="177" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="172" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="171" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="168" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="167" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="169" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="164" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9135,146 +9521,146 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="163" priority="42" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="43" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="160" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="159" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="156" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="155" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="152" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="151" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="153" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="148" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="147" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="144" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="143" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="140" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="139" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="136" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="135" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="132" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="131" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="128" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9292,7 +9678,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B70"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,7 +9893,7 @@
         <v>82</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>76</v>
@@ -9515,18 +9901,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="127" priority="78" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="79" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="78" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="79" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="80" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H1">
-    <cfRule type="cellIs" dxfId="124" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="77" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9813,7 +10199,7 @@
         <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>72</v>
@@ -9821,162 +10207,162 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 H3:H4 H6:H10">
-    <cfRule type="cellIs" dxfId="123" priority="94" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="95" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="96" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="94" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="95" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="96" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H3:H4 H6:H10">
-    <cfRule type="cellIs" dxfId="120" priority="93" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="93" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="119" priority="58" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="58" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="60" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="116" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="115" priority="54" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="55" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="54" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="55" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="112" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="111" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="108" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="107" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="104" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="103" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="100" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="99" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="96" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="95" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="92" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="91" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="88" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="87" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="84" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>